<commit_message>
Fixed wrong way of printing solution
</commit_message>
<xml_diff>
--- a/GETComp/Análise - Critério SIW.xlsx
+++ b/GETComp/Análise - Critério SIW.xlsx
@@ -9,20 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" r:id="rId1"/>
     <sheet name="ordenacao" sheetId="2" r:id="rId2"/>
     <sheet name="corteInformacao" sheetId="3" r:id="rId3"/>
     <sheet name="informacaoMaxima" sheetId="4" r:id="rId4"/>
+    <sheet name="comparacao" sheetId="5" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="82">
   <si>
     <t>model</t>
   </si>
@@ -259,6 +264,15 @@
   </si>
   <si>
     <t>Máximo de informação 100</t>
+  </si>
+  <si>
+    <t>SIW</t>
+  </si>
+  <si>
+    <t>DEGREE</t>
+  </si>
+  <si>
+    <t>RDEGREE</t>
   </si>
 </sst>
 </file>
@@ -742,8 +756,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1169,11 +1186,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1279759808"/>
-        <c:axId val="-1279756000"/>
+        <c:axId val="634127328"/>
+        <c:axId val="634127872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1279759808"/>
+        <c:axId val="634127328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,12 +1248,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1279756000"/>
+        <c:crossAx val="634127872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1279756000"/>
+        <c:axId val="634127872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1294,7 +1311,584 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1279759808"/>
+        <c:crossAx val="634127328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Corte de informação 0.001 -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> Modelo inteiro s/ solução</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>comparacao!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SIW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>comparacao!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>comparacao!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.73841</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.1417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.6768</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.184600000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.603000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>comparacao!$E$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DEGREE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>comparacao!$D$8:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>comparacao!$E$8:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.73841</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.1417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.6768</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.184600000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.603000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>comparacao!$E$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RDEGREE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>comparacao!$D$14:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>comparacao!$E$14:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.3520000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.919899999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.758099999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.257199999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.483600000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="801569376"/>
+        <c:axId val="801573184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="801569376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="801573184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="801573184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="801569376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1742,11 +2336,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1279757088"/>
-        <c:axId val="-1279754912"/>
+        <c:axId val="634131136"/>
+        <c:axId val="634130592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1279757088"/>
+        <c:axId val="634131136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1804,12 +2398,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1279754912"/>
+        <c:crossAx val="634130592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1279754912"/>
+        <c:axId val="634130592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,7 +2461,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1279757088"/>
+        <c:crossAx val="634131136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2283,11 +2877,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1279751648"/>
-        <c:axId val="-1279747296"/>
+        <c:axId val="634132768"/>
+        <c:axId val="634133312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1279751648"/>
+        <c:axId val="634132768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2345,12 +2939,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1279747296"/>
+        <c:crossAx val="634133312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1279747296"/>
+        <c:axId val="634133312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2408,7 +3002,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1279751648"/>
+        <c:crossAx val="634132768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2824,11 +3418,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1215105152"/>
-        <c:axId val="-1291598704"/>
+        <c:axId val="634134944"/>
+        <c:axId val="634135488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1215105152"/>
+        <c:axId val="634134944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2886,12 +3480,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1291598704"/>
+        <c:crossAx val="634135488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1291598704"/>
+        <c:axId val="634135488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2949,7 +3543,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1215105152"/>
+        <c:crossAx val="634134944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3347,11 +3941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1279747840"/>
-        <c:axId val="-1279746208"/>
+        <c:axId val="462005840"/>
+        <c:axId val="462006384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1279747840"/>
+        <c:axId val="462005840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3409,12 +4003,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1279746208"/>
+        <c:crossAx val="462006384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1279746208"/>
+        <c:axId val="462006384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3472,7 +4066,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1279747840"/>
+        <c:crossAx val="462005840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3906,11 +4500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1456425920"/>
-        <c:axId val="-1456425376"/>
+        <c:axId val="638855408"/>
+        <c:axId val="638861936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1456425920"/>
+        <c:axId val="638855408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3968,12 +4562,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1456425376"/>
+        <c:crossAx val="638861936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1456425376"/>
+        <c:axId val="638861936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4031,7 +4625,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1456425920"/>
+        <c:crossAx val="638855408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4465,11 +5059,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1275648928"/>
-        <c:axId val="-1275645664"/>
+        <c:axId val="638855952"/>
+        <c:axId val="638857040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1275648928"/>
+        <c:axId val="638855952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4527,12 +5121,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1275645664"/>
+        <c:crossAx val="638857040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1275645664"/>
+        <c:axId val="638857040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4590,7 +5184,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1275648928"/>
+        <c:crossAx val="638855952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5020,11 +5614,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1275645120"/>
-        <c:axId val="-1275658176"/>
+        <c:axId val="638859216"/>
+        <c:axId val="638867376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1275645120"/>
+        <c:axId val="638859216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5082,12 +5676,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1275658176"/>
+        <c:crossAx val="638867376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1275658176"/>
+        <c:axId val="638867376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5145,7 +5739,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1275645120"/>
+        <c:crossAx val="638859216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5575,11 +6169,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1275644032"/>
-        <c:axId val="-1275644576"/>
+        <c:axId val="638858128"/>
+        <c:axId val="638854320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1275644032"/>
+        <c:axId val="638858128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5637,12 +6231,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1275644576"/>
+        <c:crossAx val="638854320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1275644576"/>
+        <c:axId val="638854320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5700,7 +6294,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1275644032"/>
+        <c:crossAx val="638858128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5792,6 +6386,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6727,6 +7361,582 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="250">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="250">
   <cs:axisTitle>
@@ -11615,6 +12825,355 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4761</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Gráfico 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="dados"/>
+      <sheetName val="ordenado"/>
+      <sheetName val="corteInformacao"/>
+      <sheetName val="informacaoMaxima"/>
+      <sheetName val="Plan4"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Modelo inteiro sem solução</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>5</v>
+          </cell>
+          <cell r="B4">
+            <v>8.3520000000000003</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>15</v>
+          </cell>
+          <cell r="B5">
+            <v>18.919899999999998</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>30</v>
+          </cell>
+          <cell r="B6">
+            <v>31.758099999999999</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>50</v>
+          </cell>
+          <cell r="B7">
+            <v>43.257199999999997</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>100</v>
+          </cell>
+          <cell r="B8">
+            <v>61.483600000000003</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Modelo fracionário</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>5</v>
+          </cell>
+          <cell r="B11">
+            <v>7.1715400000000002</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>15</v>
+          </cell>
+          <cell r="B12">
+            <v>16.209900000000001</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>30</v>
+          </cell>
+          <cell r="B13">
+            <v>24.1816</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>50</v>
+          </cell>
+          <cell r="B14">
+            <v>30.613399999999999</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>100</v>
+          </cell>
+          <cell r="B15">
+            <v>43.427300000000002</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v>Modelo inteiro com solução</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>5</v>
+          </cell>
+          <cell r="B18">
+            <v>23.700700000000001</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>15</v>
+          </cell>
+          <cell r="B19">
+            <v>37.258699999999997</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>30</v>
+          </cell>
+          <cell r="B20">
+            <v>47.0182</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>50</v>
+          </cell>
+          <cell r="B21">
+            <v>54.4328</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>100</v>
+          </cell>
+          <cell r="B22">
+            <v>68.028999999999996</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="dados"/>
+      <sheetName val="ordenacao"/>
+      <sheetName val="corteiInformacao"/>
+      <sheetName val="maximoInformacao"/>
+      <sheetName val="desk"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Modelo fracionário</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>5</v>
+          </cell>
+          <cell r="B4">
+            <v>7.1715400000000002</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>15</v>
+          </cell>
+          <cell r="B5">
+            <v>16.209900000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>30</v>
+          </cell>
+          <cell r="B6">
+            <v>24.1816</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>50</v>
+          </cell>
+          <cell r="B7">
+            <v>30.613399999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>100</v>
+          </cell>
+          <cell r="B8">
+            <v>43.427300000000002</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Modelo inteiro sem solução</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>5</v>
+          </cell>
+          <cell r="B11">
+            <v>4.73841</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>15</v>
+          </cell>
+          <cell r="B12">
+            <v>14.1417</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>30</v>
+          </cell>
+          <cell r="B13">
+            <v>27.6768</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>50</v>
+          </cell>
+          <cell r="B14">
+            <v>41.184600000000003</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>100</v>
+          </cell>
+          <cell r="B15">
+            <v>61.603000000000002</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v>Modelo inteiro com solução</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>5</v>
+          </cell>
+          <cell r="B18">
+            <v>23.700700000000001</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>15</v>
+          </cell>
+          <cell r="B19">
+            <v>37.258699999999997</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>30</v>
+          </cell>
+          <cell r="B20">
+            <v>47.0182</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>50</v>
+          </cell>
+          <cell r="B21">
+            <v>54.4328</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>100</v>
+          </cell>
+          <cell r="B22">
+            <v>68.028999999999996</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -21479,8 +23038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21501,48 +23060,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -21773,26 +23332,26 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -22023,26 +23582,26 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2" t="s">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -22274,6 +23833,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D16:F16"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="G9:I9"/>
@@ -22282,14 +23849,6 @@
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="J16:L16"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D16:F16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -22300,7 +23859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
@@ -22322,58 +23881,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -22611,31 +24170,31 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2" t="s">
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -22873,31 +24432,31 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2" t="s">
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -23139,6 +24698,13 @@
     <sortCondition ref="A1"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O1"/>
@@ -23152,15 +24718,168 @@
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="M2:O2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4.73841</v>
+      </c>
+    </row>
+    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2">
+        <v>14.1417</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2">
+        <v>27.6768</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>50</v>
+      </c>
+      <c r="E5" s="2">
+        <v>41.184600000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2">
+        <v>61.603000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>4.73841</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>14.1417</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="E10">
+        <v>27.6768</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>41.184600000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>61.603000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>8.3520000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>18.919899999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <v>31.758099999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <v>50</v>
+      </c>
+      <c r="E17">
+        <v>43.257199999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <v>100</v>
+      </c>
+      <c r="E18">
+        <v>61.483600000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Greedy algorithm, fix criteria selection
</commit_message>
<xml_diff>
--- a/GETComp/Análise - Critério SIW.xlsx
+++ b/GETComp/Análise - Critério SIW.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,6 @@
     <sheet name="informacaoMaxima" sheetId="4" r:id="rId4"/>
     <sheet name="comparacao" sheetId="5" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -869,7 +865,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1186,11 +1181,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="634127328"/>
-        <c:axId val="634127872"/>
+        <c:axId val="-821728784"/>
+        <c:axId val="-821734224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="634127328"/>
+        <c:axId val="-821728784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,12 +1243,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634127872"/>
+        <c:crossAx val="-821734224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="634127872"/>
+        <c:axId val="-821734224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1311,7 +1306,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634127328"/>
+        <c:crossAx val="-821728784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1335,7 +1330,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1763,11 +1757,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="801569376"/>
-        <c:axId val="801573184"/>
+        <c:axId val="-748278240"/>
+        <c:axId val="-748277696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="801569376"/>
+        <c:axId val="-748278240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1825,12 +1819,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="801573184"/>
+        <c:crossAx val="-748277696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="801573184"/>
+        <c:axId val="-748277696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1888,7 +1882,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="801569376"/>
+        <c:crossAx val="-748278240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2019,7 +2013,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2336,11 +2329,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="634131136"/>
-        <c:axId val="634130592"/>
+        <c:axId val="-820475552"/>
+        <c:axId val="-820473920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="634131136"/>
+        <c:axId val="-820475552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2398,12 +2391,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634130592"/>
+        <c:crossAx val="-820473920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="634130592"/>
+        <c:axId val="-820473920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2461,7 +2454,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634131136"/>
+        <c:crossAx val="-820475552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2560,7 +2553,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2877,11 +2869,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="634132768"/>
-        <c:axId val="634133312"/>
+        <c:axId val="-833686448"/>
+        <c:axId val="-833682096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="634132768"/>
+        <c:axId val="-833686448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2939,12 +2931,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634133312"/>
+        <c:crossAx val="-833682096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="634133312"/>
+        <c:axId val="-833682096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3002,7 +2994,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634132768"/>
+        <c:crossAx val="-833686448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3101,7 +3093,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3418,11 +3409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="634134944"/>
-        <c:axId val="634135488"/>
+        <c:axId val="-755918816"/>
+        <c:axId val="-1099987680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="634134944"/>
+        <c:axId val="-755918816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3480,12 +3471,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634135488"/>
+        <c:crossAx val="-1099987680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="634135488"/>
+        <c:axId val="-1099987680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3543,7 +3534,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="634134944"/>
+        <c:crossAx val="-755918816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3642,7 +3633,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3941,11 +3931,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="462005840"/>
-        <c:axId val="462006384"/>
+        <c:axId val="-748271712"/>
+        <c:axId val="-748267904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="462005840"/>
+        <c:axId val="-748271712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4003,12 +3993,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="462006384"/>
+        <c:crossAx val="-748267904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="462006384"/>
+        <c:axId val="-748267904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4066,7 +4056,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="462005840"/>
+        <c:crossAx val="-748271712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4090,7 +4080,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4201,7 +4190,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4500,11 +4488,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="638855408"/>
-        <c:axId val="638861936"/>
+        <c:axId val="-748280416"/>
+        <c:axId val="-748267360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="638855408"/>
+        <c:axId val="-748280416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4562,12 +4550,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="638861936"/>
+        <c:crossAx val="-748267360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="638861936"/>
+        <c:axId val="-748267360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4625,7 +4613,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="638855408"/>
+        <c:crossAx val="-748280416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4649,7 +4637,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4760,7 +4747,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5059,11 +5045,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="638855952"/>
-        <c:axId val="638857040"/>
+        <c:axId val="-748270080"/>
+        <c:axId val="-748273888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="638855952"/>
+        <c:axId val="-748270080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5121,12 +5107,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="638857040"/>
+        <c:crossAx val="-748273888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="638857040"/>
+        <c:axId val="-748273888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5184,7 +5170,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="638855952"/>
+        <c:crossAx val="-748270080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5208,7 +5194,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5315,7 +5300,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5614,11 +5598,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="638859216"/>
-        <c:axId val="638867376"/>
+        <c:axId val="-748275520"/>
+        <c:axId val="-748278784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="638859216"/>
+        <c:axId val="-748275520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5676,12 +5660,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="638867376"/>
+        <c:crossAx val="-748278784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="638867376"/>
+        <c:axId val="-748278784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5739,7 +5723,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="638859216"/>
+        <c:crossAx val="-748275520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5763,7 +5747,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5870,7 +5853,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6169,11 +6151,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="638858128"/>
-        <c:axId val="638854320"/>
+        <c:axId val="-748279872"/>
+        <c:axId val="-748265184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="638858128"/>
+        <c:axId val="-748279872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6231,12 +6213,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="638854320"/>
+        <c:crossAx val="-748265184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="638854320"/>
+        <c:axId val="-748265184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6294,7 +6276,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="638858128"/>
+        <c:crossAx val="-748279872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6318,7 +6300,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12860,320 +12841,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="dados"/>
-      <sheetName val="ordenado"/>
-      <sheetName val="corteInformacao"/>
-      <sheetName val="informacaoMaxima"/>
-      <sheetName val="Plan4"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>Modelo inteiro sem solução</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>5</v>
-          </cell>
-          <cell r="B4">
-            <v>8.3520000000000003</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>15</v>
-          </cell>
-          <cell r="B5">
-            <v>18.919899999999998</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>30</v>
-          </cell>
-          <cell r="B6">
-            <v>31.758099999999999</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>50</v>
-          </cell>
-          <cell r="B7">
-            <v>43.257199999999997</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>100</v>
-          </cell>
-          <cell r="B8">
-            <v>61.483600000000003</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>Modelo fracionário</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>5</v>
-          </cell>
-          <cell r="B11">
-            <v>7.1715400000000002</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>15</v>
-          </cell>
-          <cell r="B12">
-            <v>16.209900000000001</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>30</v>
-          </cell>
-          <cell r="B13">
-            <v>24.1816</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>50</v>
-          </cell>
-          <cell r="B14">
-            <v>30.613399999999999</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>100</v>
-          </cell>
-          <cell r="B15">
-            <v>43.427300000000002</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>Modelo inteiro com solução</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>5</v>
-          </cell>
-          <cell r="B18">
-            <v>23.700700000000001</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>15</v>
-          </cell>
-          <cell r="B19">
-            <v>37.258699999999997</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>30</v>
-          </cell>
-          <cell r="B20">
-            <v>47.0182</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>50</v>
-          </cell>
-          <cell r="B21">
-            <v>54.4328</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>100</v>
-          </cell>
-          <cell r="B22">
-            <v>68.028999999999996</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="dados"/>
-      <sheetName val="ordenacao"/>
-      <sheetName val="corteiInformacao"/>
-      <sheetName val="maximoInformacao"/>
-      <sheetName val="desk"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>Modelo fracionário</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>5</v>
-          </cell>
-          <cell r="B4">
-            <v>7.1715400000000002</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>15</v>
-          </cell>
-          <cell r="B5">
-            <v>16.209900000000001</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>30</v>
-          </cell>
-          <cell r="B6">
-            <v>24.1816</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>50</v>
-          </cell>
-          <cell r="B7">
-            <v>30.613399999999999</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>100</v>
-          </cell>
-          <cell r="B8">
-            <v>43.427300000000002</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>Modelo inteiro sem solução</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>5</v>
-          </cell>
-          <cell r="B11">
-            <v>4.73841</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>15</v>
-          </cell>
-          <cell r="B12">
-            <v>14.1417</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>30</v>
-          </cell>
-          <cell r="B13">
-            <v>27.6768</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>50</v>
-          </cell>
-          <cell r="B14">
-            <v>41.184600000000003</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>100</v>
-          </cell>
-          <cell r="B15">
-            <v>61.603000000000002</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>Modelo inteiro com solução</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>5</v>
-          </cell>
-          <cell r="B18">
-            <v>23.700700000000001</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>15</v>
-          </cell>
-          <cell r="B19">
-            <v>37.258699999999997</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>30</v>
-          </cell>
-          <cell r="B20">
-            <v>47.0182</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>50</v>
-          </cell>
-          <cell r="B21">
-            <v>54.4328</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>100</v>
-          </cell>
-          <cell r="B22">
-            <v>68.028999999999996</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -13439,8 +13106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23833,6 +23500,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J16:L16"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A9:C9"/>
@@ -23841,14 +23516,6 @@
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J16:L16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -24698,13 +24365,6 @@
     <sortCondition ref="A1"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O1"/>
@@ -24718,6 +24378,13 @@
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="M2:O2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -24728,7 +24395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>

</xml_diff>